<commit_message>
For Actitime Login Page - Admin n User Login
</commit_message>
<xml_diff>
--- a/result/Summary.xlsx
+++ b/result/Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView windowHeight="4740" windowWidth="13875" xWindow="0" yWindow="2520"/>
+    <workbookView windowHeight="4200" windowWidth="13875" xWindow="0" yWindow="2520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -116,6 +116,32 @@
               </a:solidFill>
             </c:spPr>
           </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.1800588058347708E-3"/>
+                  <c:y val="-0.17721530762836482"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="inEnd"/>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.1797296932604986E-3"/>
+                  <c:y val="-0.20253178014670264"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="inEnd"/>
+              <c:showVal val="1"/>
+            </c:dLbl>
+            <c:dLblPos val="inEnd"/>
+            <c:showVal val="1"/>
+          </c:dLbls>
           <c:cat>
             <c:strRef>
               <c:f>Sheet1!$A$1:$B$1</c:f>
@@ -140,31 +166,31 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="51220480"/>
-        <c:axId val="51222016"/>
+        <c:axId val="64000768"/>
+        <c:axId val="64002304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="51220480"/>
+        <c:axId val="64000768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51222016"/>
+        <c:crossAx val="64002304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51222016"/>
+        <c:axId val="64002304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -172,7 +198,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51220480"/>
+        <c:crossAx val="64000768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -185,7 +211,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" footer="0.30000000000000004" header="0.30000000000000004" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011"/>
+    <c:pageMargins b="0.75000000000000044" footer="0.30000000000000021" header="0.30000000000000021" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -514,7 +540,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -533,7 +559,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>

</xml_diff>